<commit_message>
Filter and aggregation for life stages (zooplankton). Copy to clipboard for analysis data. Etc.
</commit_message>
<xml_diff>
--- a/toolbox_data/parsers/sharkweb_phytoplankton_parser.xlsx
+++ b/toolbox_data/parsers/sharkweb_phytoplankton_parser.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="2800" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2660" yWindow="40" windowWidth="29740" windowHeight="20260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="pp_import_matrix.txt" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="224">
   <si>
     <t>Node level</t>
   </si>
@@ -75,9 +75,6 @@
     <t>PEG_TROPHY</t>
   </si>
   <si>
-    <t>DT_CLASS</t>
-  </si>
-  <si>
     <t>REP_LATIT</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>$Text('Unit')</t>
   </si>
   <si>
-    <t>CLASS</t>
-  </si>
-  <si>
     <t>$Text('Sample identifier')</t>
   </si>
   <si>
@@ -237,9 +231,6 @@
     <t>trophy</t>
   </si>
   <si>
-    <t>dt_class</t>
-  </si>
-  <si>
     <t>peg_trophy</t>
   </si>
   <si>
@@ -396,9 +387,6 @@
     <t>$Text('Trofi') if $Text('Trofi') else 'NS'</t>
   </si>
   <si>
-    <t>Klass (Dyntaxa)</t>
-  </si>
-  <si>
     <t>Planktongrupp</t>
   </si>
   <si>
@@ -435,9 +423,6 @@
     <t>$Text(u'Mätenhet')</t>
   </si>
   <si>
-    <t>$Species($Text(u'Använt taxonnamn'), key='Class')</t>
-  </si>
-  <si>
     <t>$PlanktonGroup($Text(u'Använt taxonnamn'))</t>
   </si>
   <si>
@@ -474,9 +459,6 @@
     <t>$PlanktonGroup($Text('Used taxon name'))</t>
   </si>
   <si>
-    <t>$Species($Text('Used taxon name'), key='Class')</t>
-  </si>
-  <si>
     <t>windows-1252</t>
   </si>
   <si>
@@ -558,9 +540,6 @@
     <t>Plankton group</t>
   </si>
   <si>
-    <t>Class (Dyntaxa)</t>
-  </si>
-  <si>
     <t>Trophy (PEG)</t>
   </si>
   <si>
@@ -592,6 +571,126 @@
   </si>
   <si>
     <t>Sharkweb english (carbon calculated)</t>
+  </si>
+  <si>
+    <t>taxon_id</t>
+  </si>
+  <si>
+    <t>$Text('Taxon_id')</t>
+  </si>
+  <si>
+    <t>$Text('Taxon-id')</t>
+  </si>
+  <si>
+    <t>Taxon_id</t>
+  </si>
+  <si>
+    <t>Taxon-id</t>
+  </si>
+  <si>
+    <t>kingdom</t>
+  </si>
+  <si>
+    <t>$Text('Kingdom')</t>
+  </si>
+  <si>
+    <t>$Text('Rike')</t>
+  </si>
+  <si>
+    <t>Kingdom</t>
+  </si>
+  <si>
+    <t>Rike</t>
+  </si>
+  <si>
+    <t>phylum</t>
+  </si>
+  <si>
+    <t>$Text('Phylum')</t>
+  </si>
+  <si>
+    <t>$Text('Stam')</t>
+  </si>
+  <si>
+    <t>Phylum</t>
+  </si>
+  <si>
+    <t>Stam</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>$Text('Order')</t>
+  </si>
+  <si>
+    <t>$Text('Ordning')</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Ordning</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>$Text('Family')</t>
+  </si>
+  <si>
+    <t>$Text('Familj')</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Familj</t>
+  </si>
+  <si>
+    <t>genus</t>
+  </si>
+  <si>
+    <t>$Text('Genus')</t>
+  </si>
+  <si>
+    <t>$Text(u'Släkte')</t>
+  </si>
+  <si>
+    <t>Genus</t>
+  </si>
+  <si>
+    <t>Släkte</t>
+  </si>
+  <si>
+    <t>parent_taxa</t>
+  </si>
+  <si>
+    <t>$Text('Parent taxa')</t>
+  </si>
+  <si>
+    <t>$Text(u'Föräldrataxa')</t>
+  </si>
+  <si>
+    <t>Parent taxa</t>
+  </si>
+  <si>
+    <t>Föräldrataxa</t>
+  </si>
+  <si>
+    <t>reported_taxon_name</t>
+  </si>
+  <si>
+    <t>$Text('Reported taxon name')</t>
+  </si>
+  <si>
+    <t>$Text('Rapporterat taxon-namn')</t>
+  </si>
+  <si>
+    <t>Reported taxon name</t>
+  </si>
+  <si>
+    <t>Rapporterat taxon-namn</t>
   </si>
 </sst>
 </file>
@@ -653,8 +752,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="239">
+  <cellStyleXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -898,7 +1013,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="239">
+  <cellStyles count="255">
     <cellStyle name="Följd hyperlänk" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="6" builtinId="9" hidden="1"/>
@@ -1018,6 +1133,14 @@
     <cellStyle name="Följd hyperlänk" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="236" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="254" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="5" builtinId="8" hidden="1"/>
@@ -1137,6 +1260,14 @@
     <cellStyle name="Hyperlänk" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="235" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="253" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1466,10 +1597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="G6" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1491,108 +1622,108 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" t="s">
         <v>89</v>
       </c>
-      <c r="E1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F1" t="s">
-        <v>92</v>
-      </c>
       <c r="G1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="I1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1609,10 +1740,10 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -1629,59 +1760,59 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E8" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F8" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="G8" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I10" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="J10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="K10" t="s">
         <v>16</v>
@@ -1689,31 +1820,31 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I11" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="J11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K11" t="s">
         <v>2</v>
@@ -1721,31 +1852,31 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E12" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I12" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K12" t="s">
         <v>3</v>
@@ -1753,63 +1884,63 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E14" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F14" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G14" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I14" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="J14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="K14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E15" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F15" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G15" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I15" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="J15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K15" t="s">
         <v>5</v>
@@ -1817,95 +1948,95 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D16" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E16" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D17" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E17" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I17" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="J17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I18" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="J18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K18" t="s">
         <v>4</v>
@@ -1913,63 +2044,63 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I20" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F21" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G21" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I21" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="K21" t="s">
         <v>6</v>
@@ -1977,31 +2108,31 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I22" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="J22" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K22" t="s">
         <v>7</v>
@@ -2009,31 +2140,31 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I23" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K23" t="s">
         <v>8</v>
@@ -2041,31 +2172,31 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F25" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G25" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I25" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="J25" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K25" t="s">
         <v>9</v>
@@ -2073,31 +2204,31 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E26" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F26" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G26" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="I26" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="J26" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K26" t="s">
         <v>12</v>
@@ -2105,31 +2236,31 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E27" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I27" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K27" t="s">
         <v>11</v>
@@ -2137,31 +2268,31 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I28" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="J28" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K28" t="s">
         <v>10</v>
@@ -2169,257 +2300,257 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>158</v>
+        <v>41</v>
       </c>
       <c r="E29" t="s">
-        <v>158</v>
+        <v>41</v>
       </c>
       <c r="F29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I29" t="s">
-        <v>176</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>110</v>
+        <v>171</v>
+      </c>
+      <c r="J29" t="s">
+        <v>103</v>
       </c>
       <c r="K29" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="E30" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="F30" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="G30" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="I30" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="J30" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="K30" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C31" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F31" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G31" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I31" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="J31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" t="s">
         <v>79</v>
       </c>
-      <c r="C32" t="s">
-        <v>81</v>
-      </c>
       <c r="D32" t="s">
-        <v>150</v>
+        <v>36</v>
       </c>
       <c r="E32" t="s">
-        <v>150</v>
+        <v>36</v>
       </c>
       <c r="F32" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="G32" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="I32" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="J32" t="s">
-        <v>126</v>
+        <v>177</v>
       </c>
       <c r="K32" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C33" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" t="s">
-        <v>153</v>
+        <v>79</v>
       </c>
       <c r="E33" t="s">
-        <v>153</v>
-      </c>
-      <c r="F33" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="G33" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="I33" t="s">
-        <v>180</v>
+        <v>31</v>
       </c>
       <c r="J33" t="s">
-        <v>127</v>
+        <v>31</v>
       </c>
       <c r="K33" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C34" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F34" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="G34" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="I34" t="s">
-        <v>181</v>
+        <v>32</v>
       </c>
       <c r="J34" t="s">
-        <v>184</v>
+        <v>32</v>
       </c>
       <c r="K34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
-      <c r="A35" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" t="s">
-        <v>82</v>
-      </c>
-      <c r="E35" t="s">
-        <v>155</v>
-      </c>
-      <c r="G35" t="s">
-        <v>156</v>
-      </c>
-      <c r="I35" t="s">
-        <v>33</v>
-      </c>
-      <c r="J35" t="s">
-        <v>33</v>
-      </c>
-      <c r="K35" t="s">
-        <v>33</v>
-      </c>
-    </row>
     <row r="36" spans="1:11">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
         <v>78</v>
       </c>
-      <c r="C36" t="s">
-        <v>82</v>
+      <c r="D36" t="s">
+        <v>23</v>
       </c>
       <c r="E36" t="s">
-        <v>154</v>
+        <v>23</v>
+      </c>
+      <c r="F36" t="s">
+        <v>23</v>
       </c>
       <c r="G36" t="s">
-        <v>157</v>
+        <v>23</v>
       </c>
       <c r="I36" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="J36" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="K36" t="s">
-        <v>34</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" t="s">
+        <v>37</v>
+      </c>
+      <c r="F37" t="s">
+        <v>132</v>
+      </c>
+      <c r="G37" t="s">
+        <v>132</v>
+      </c>
+      <c r="I37" t="s">
+        <v>175</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K37" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D38" t="s">
         <v>24</v>
@@ -2428,105 +2559,329 @@
         <v>24</v>
       </c>
       <c r="F38" t="s">
-        <v>24</v>
+        <v>133</v>
       </c>
       <c r="G38" t="s">
-        <v>24</v>
+        <v>133</v>
       </c>
       <c r="I38" t="s">
-        <v>107</v>
+        <v>176</v>
       </c>
       <c r="J38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K38" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" t="s">
-        <v>39</v>
-      </c>
-      <c r="E39" t="s">
-        <v>39</v>
-      </c>
-      <c r="F39" t="s">
-        <v>136</v>
-      </c>
-      <c r="G39" t="s">
-        <v>136</v>
-      </c>
-      <c r="I39" t="s">
-        <v>182</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K39" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="E40" t="s">
-        <v>25</v>
-      </c>
-      <c r="F40" t="s">
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="G40" t="s">
-        <v>137</v>
-      </c>
-      <c r="I40" t="s">
-        <v>183</v>
-      </c>
-      <c r="J40" t="s">
-        <v>109</v>
-      </c>
-      <c r="K40" t="s">
-        <v>15</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E42" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G42" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>184</v>
+      </c>
+      <c r="C44" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" t="s">
+        <v>185</v>
       </c>
       <c r="E44" t="s">
+        <v>185</v>
+      </c>
+      <c r="F44" t="s">
+        <v>186</v>
+      </c>
+      <c r="G44" t="s">
+        <v>186</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G44" t="s">
+      <c r="J44" t="s">
         <v>188</v>
+      </c>
+      <c r="K44" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>189</v>
+      </c>
+      <c r="C45" t="s">
+        <v>78</v>
+      </c>
+      <c r="D45" t="s">
+        <v>190</v>
+      </c>
+      <c r="E45" t="s">
+        <v>190</v>
+      </c>
+      <c r="F45" t="s">
+        <v>191</v>
+      </c>
+      <c r="G45" t="s">
+        <v>191</v>
+      </c>
+      <c r="I45" t="s">
+        <v>192</v>
+      </c>
+      <c r="J45" t="s">
+        <v>193</v>
+      </c>
+      <c r="K45" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>194</v>
+      </c>
+      <c r="C46" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" t="s">
+        <v>195</v>
+      </c>
+      <c r="E46" t="s">
+        <v>195</v>
+      </c>
+      <c r="F46" t="s">
+        <v>196</v>
+      </c>
+      <c r="G46" t="s">
+        <v>196</v>
+      </c>
+      <c r="I46" t="s">
+        <v>197</v>
+      </c>
+      <c r="J46" t="s">
+        <v>198</v>
+      </c>
+      <c r="K46" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" t="s">
+        <v>152</v>
+      </c>
+      <c r="E47" t="s">
+        <v>152</v>
+      </c>
+      <c r="F47" t="s">
+        <v>120</v>
+      </c>
+      <c r="G47" t="s">
+        <v>120</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" t="s">
+        <v>199</v>
+      </c>
+      <c r="C48" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" t="s">
+        <v>200</v>
+      </c>
+      <c r="E48" t="s">
+        <v>200</v>
+      </c>
+      <c r="F48" t="s">
+        <v>201</v>
+      </c>
+      <c r="G48" t="s">
+        <v>201</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" t="s">
+        <v>204</v>
+      </c>
+      <c r="C49" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" t="s">
+        <v>205</v>
+      </c>
+      <c r="E49" t="s">
+        <v>205</v>
+      </c>
+      <c r="F49" t="s">
+        <v>206</v>
+      </c>
+      <c r="G49" t="s">
+        <v>206</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" t="s">
+        <v>209</v>
+      </c>
+      <c r="C50" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" t="s">
+        <v>210</v>
+      </c>
+      <c r="E50" t="s">
+        <v>210</v>
+      </c>
+      <c r="F50" t="s">
+        <v>211</v>
+      </c>
+      <c r="G50" t="s">
+        <v>211</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J50" t="s">
+        <v>213</v>
+      </c>
+      <c r="K50" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
+        <v>214</v>
+      </c>
+      <c r="C51" t="s">
+        <v>78</v>
+      </c>
+      <c r="D51" t="s">
+        <v>215</v>
+      </c>
+      <c r="E51" t="s">
+        <v>215</v>
+      </c>
+      <c r="F51" t="s">
+        <v>216</v>
+      </c>
+      <c r="G51" t="s">
+        <v>216</v>
+      </c>
+      <c r="I51" t="s">
+        <v>217</v>
+      </c>
+      <c r="J51" t="s">
+        <v>218</v>
+      </c>
+      <c r="K51" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" t="s">
+        <v>219</v>
+      </c>
+      <c r="C52" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" t="s">
+        <v>220</v>
+      </c>
+      <c r="E52" t="s">
+        <v>220</v>
+      </c>
+      <c r="F52" t="s">
+        <v>221</v>
+      </c>
+      <c r="G52" t="s">
+        <v>221</v>
+      </c>
+      <c r="I52" t="s">
+        <v>222</v>
+      </c>
+      <c r="J52" t="s">
+        <v>223</v>
+      </c>
+      <c r="K52" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preparing for the next public release. Work in progress...
</commit_message>
<xml_diff>
--- a/toolbox_data/parsers/sharkweb_phytoplankton_parser.xlsx
+++ b/toolbox_data/parsers/sharkweb_phytoplankton_parser.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6500" yWindow="0" windowWidth="29740" windowHeight="20260" tabRatio="500"/>
+    <workbookView xWindow="4460" yWindow="0" windowWidth="29740" windowHeight="20260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="pp_import_matrix.txt" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="232">
   <si>
     <t>Node level</t>
   </si>
@@ -216,9 +216,6 @@
     <t>analytical_laboratory_code</t>
   </si>
   <si>
-    <t>taxon_name</t>
-  </si>
-  <si>
     <t>species_flag_code</t>
   </si>
   <si>
@@ -564,9 +561,6 @@
     <t>Sharkweb english (carbon calculated)</t>
   </si>
   <si>
-    <t>taxon_id</t>
-  </si>
-  <si>
     <t>$Text('Taxon_id')</t>
   </si>
   <si>
@@ -669,9 +663,6 @@
     <t>Föräldrataxa</t>
   </si>
   <si>
-    <t>reported_taxon_name</t>
-  </si>
-  <si>
     <t>$Text('Reported taxon name')</t>
   </si>
   <si>
@@ -694,6 +685,36 @@
   </si>
   <si>
     <t>$Sizeclass($Text(u'Använt taxonnamn'), $Text('Storleksklass'), key='Trophy')</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>datatype_code</t>
+  </si>
+  <si>
+    <t>$Text('Data type')</t>
+  </si>
+  <si>
+    <t>$Text('Datatyp')</t>
+  </si>
+  <si>
+    <t>Data type</t>
+  </si>
+  <si>
+    <t>Datatyp</t>
+  </si>
+  <si>
+    <t>DATATYPE</t>
+  </si>
+  <si>
+    <t>scientific_name</t>
+  </si>
+  <si>
+    <t>reported_scientific_name</t>
+  </si>
+  <si>
+    <t>dyntaxa_id</t>
   </si>
 </sst>
 </file>
@@ -755,8 +776,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="255">
+  <cellStyleXfs count="265">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1016,7 +1047,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="255">
+  <cellStyles count="265">
     <cellStyle name="Följd hyperlänk" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="6" builtinId="9" hidden="1"/>
@@ -1144,6 +1175,11 @@
     <cellStyle name="Följd hyperlänk" xfId="250" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="252" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="264" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="5" builtinId="8" hidden="1"/>
@@ -1271,6 +1307,11 @@
     <cellStyle name="Hyperlänk" xfId="249" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="251" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="263" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1600,10 +1641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1628,102 +1669,102 @@
         <v>40</v>
       </c>
       <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I1" t="s">
         <v>86</v>
       </c>
-      <c r="E1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" t="s">
-        <v>179</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>87</v>
       </c>
-      <c r="J1" t="s">
-        <v>88</v>
-      </c>
       <c r="K1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
         <v>45</v>
       </c>
       <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
         <v>81</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" t="s">
         <v>82</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J2" t="s">
         <v>82</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K2" t="s">
         <v>82</v>
-      </c>
-      <c r="G2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
         <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
         <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
         <v>48</v>
@@ -1743,7 +1784,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
         <v>49</v>
@@ -1763,7 +1804,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
@@ -1771,54 +1812,54 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>222</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>223</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>224</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>224</v>
       </c>
       <c r="F10" t="s">
-        <v>127</v>
+        <v>225</v>
       </c>
       <c r="G10" t="s">
-        <v>127</v>
+        <v>225</v>
       </c>
       <c r="I10" t="s">
-        <v>152</v>
+        <v>226</v>
       </c>
       <c r="J10" t="s">
-        <v>90</v>
-      </c>
-      <c r="K10" t="s">
-        <v>16</v>
+        <v>227</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1826,31 +1867,31 @@
         <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="G11" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="I11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K11" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1858,63 +1899,63 @@
         <v>42</v>
       </c>
       <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" t="s">
+        <v>109</v>
+      </c>
+      <c r="I12" t="s">
+        <v>152</v>
+      </c>
+      <c r="J12" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
         <v>54</v>
       </c>
-      <c r="C12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" t="s">
-        <v>136</v>
-      </c>
-      <c r="E12" t="s">
-        <v>136</v>
-      </c>
-      <c r="F12" t="s">
-        <v>111</v>
-      </c>
-      <c r="G12" t="s">
-        <v>111</v>
-      </c>
-      <c r="I12" t="s">
-        <v>154</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" t="s">
+        <v>110</v>
+      </c>
+      <c r="I13" t="s">
+        <v>153</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K13" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" t="s">
-        <v>138</v>
-      </c>
-      <c r="E14" t="s">
-        <v>138</v>
-      </c>
-      <c r="F14" t="s">
-        <v>128</v>
-      </c>
-      <c r="G14" t="s">
-        <v>128</v>
-      </c>
-      <c r="I14" t="s">
-        <v>155</v>
-      </c>
-      <c r="J14" t="s">
-        <v>93</v>
-      </c>
-      <c r="K14" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1922,31 +1963,31 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K15" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1954,31 +1995,31 @@
         <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F16" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="G16" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="I16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K16" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1986,31 +2027,31 @@
         <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -2018,63 +2059,63 @@
         <v>42</v>
       </c>
       <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" t="s">
+        <v>140</v>
+      </c>
+      <c r="E18" t="s">
+        <v>140</v>
+      </c>
+      <c r="F18" t="s">
+        <v>111</v>
+      </c>
+      <c r="G18" t="s">
+        <v>111</v>
+      </c>
+      <c r="I18" t="s">
+        <v>157</v>
+      </c>
+      <c r="J18" t="s">
+        <v>94</v>
+      </c>
+      <c r="K18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
         <v>59</v>
       </c>
-      <c r="C18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" t="s">
         <v>19</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>19</v>
       </c>
-      <c r="F18" t="s">
-        <v>113</v>
-      </c>
-      <c r="G18" t="s">
-        <v>113</v>
-      </c>
-      <c r="I18" t="s">
-        <v>159</v>
-      </c>
-      <c r="J18" t="s">
-        <v>99</v>
-      </c>
-      <c r="K18" t="s">
+      <c r="F19" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I19" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19" t="s">
+        <v>98</v>
+      </c>
+      <c r="K19" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" t="s">
-        <v>114</v>
-      </c>
-      <c r="G20" t="s">
-        <v>114</v>
-      </c>
-      <c r="I20" t="s">
-        <v>160</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="K20" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -2082,31 +2123,31 @@
         <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F21" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="G21" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="I21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K21" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -2114,31 +2155,31 @@
         <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F22" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="G22" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="I22" t="s">
-        <v>162</v>
-      </c>
-      <c r="J22" t="s">
-        <v>98</v>
+        <v>160</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="K22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -2146,63 +2187,63 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
         <v>78</v>
       </c>
       <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>114</v>
+      </c>
+      <c r="G23" t="s">
+        <v>114</v>
+      </c>
+      <c r="I23" t="s">
+        <v>161</v>
+      </c>
+      <c r="J23" t="s">
+        <v>97</v>
+      </c>
+      <c r="K23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" t="s">
         <v>20</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>20</v>
       </c>
-      <c r="F23" t="s">
-        <v>116</v>
-      </c>
-      <c r="G23" t="s">
-        <v>116</v>
-      </c>
-      <c r="I23" t="s">
-        <v>163</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="F24" t="s">
+        <v>115</v>
+      </c>
+      <c r="G24" t="s">
+        <v>115</v>
+      </c>
+      <c r="I24" t="s">
+        <v>162</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K24" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" t="s">
-        <v>117</v>
-      </c>
-      <c r="G25" t="s">
-        <v>117</v>
-      </c>
-      <c r="I25" t="s">
-        <v>164</v>
-      </c>
-      <c r="J25" t="s">
-        <v>109</v>
-      </c>
-      <c r="K25" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2210,31 +2251,31 @@
         <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>143</v>
+        <v>21</v>
       </c>
       <c r="E26" t="s">
-        <v>143</v>
+        <v>21</v>
       </c>
       <c r="F26" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="G26" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="I26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J26" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="K26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -2242,31 +2283,31 @@
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>229</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="E27" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="F27" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="G27" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="I27" t="s">
-        <v>167</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>101</v>
+        <v>164</v>
+      </c>
+      <c r="J27" t="s">
+        <v>99</v>
       </c>
       <c r="K27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2274,31 +2315,31 @@
         <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>165</v>
       </c>
       <c r="E28" t="s">
-        <v>22</v>
+        <v>165</v>
       </c>
       <c r="F28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I28" t="s">
-        <v>168</v>
-      </c>
-      <c r="J28" t="s">
-        <v>102</v>
+        <v>166</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="K28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2306,31 +2347,31 @@
         <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="F29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I29" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J29" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K29" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -2338,31 +2379,31 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D30" t="s">
-        <v>144</v>
+        <v>41</v>
       </c>
       <c r="E30" t="s">
-        <v>144</v>
+        <v>41</v>
       </c>
       <c r="F30" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="G30" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="I30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J30" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="K30" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2370,31 +2411,31 @@
         <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D31" t="s">
-        <v>223</v>
+        <v>143</v>
       </c>
       <c r="E31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F31" t="s">
-        <v>224</v>
+        <v>133</v>
       </c>
       <c r="G31" t="s">
-        <v>224</v>
+        <v>133</v>
       </c>
       <c r="I31" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K31" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2402,31 +2443,31 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" t="s">
         <v>77</v>
       </c>
-      <c r="C32" t="s">
-        <v>79</v>
-      </c>
       <c r="D32" t="s">
-        <v>36</v>
+        <v>220</v>
       </c>
       <c r="E32" t="s">
-        <v>36</v>
+        <v>145</v>
       </c>
       <c r="F32" t="s">
-        <v>124</v>
+        <v>221</v>
       </c>
       <c r="G32" t="s">
-        <v>124</v>
+        <v>221</v>
       </c>
       <c r="I32" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J32" t="s">
-        <v>176</v>
+        <v>122</v>
       </c>
       <c r="K32" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -2434,25 +2475,31 @@
         <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
       </c>
       <c r="E33" t="s">
-        <v>148</v>
+        <v>36</v>
+      </c>
+      <c r="F33" t="s">
+        <v>123</v>
       </c>
       <c r="G33" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="I33" t="s">
-        <v>31</v>
+        <v>172</v>
       </c>
       <c r="J33" t="s">
-        <v>31</v>
+        <v>175</v>
       </c>
       <c r="K33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2460,57 +2507,51 @@
         <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E34" t="s">
         <v>147</v>
       </c>
       <c r="G34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J34" t="s">
+        <v>31</v>
+      </c>
+      <c r="K34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" t="s">
+        <v>146</v>
+      </c>
+      <c r="G35" t="s">
+        <v>149</v>
+      </c>
+      <c r="I35" t="s">
         <v>32</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J35" t="s">
         <v>32</v>
       </c>
-      <c r="K34" t="s">
+      <c r="K35" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" t="s">
-        <v>78</v>
-      </c>
-      <c r="D36" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" t="s">
-        <v>23</v>
-      </c>
-      <c r="F36" t="s">
-        <v>23</v>
-      </c>
-      <c r="G36" t="s">
-        <v>23</v>
-      </c>
-      <c r="I36" t="s">
-        <v>104</v>
-      </c>
-      <c r="J36" t="s">
-        <v>104</v>
-      </c>
-      <c r="K36" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2518,31 +2559,31 @@
         <v>44</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D37" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E37" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="F37" t="s">
-        <v>132</v>
+        <v>23</v>
       </c>
       <c r="G37" t="s">
-        <v>132</v>
+        <v>23</v>
       </c>
       <c r="I37" t="s">
-        <v>174</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
+      </c>
+      <c r="J37" t="s">
+        <v>103</v>
       </c>
       <c r="K37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2550,85 +2591,85 @@
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C38" t="s">
         <v>78</v>
       </c>
       <c r="D38" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" t="s">
+        <v>131</v>
+      </c>
+      <c r="G38" t="s">
+        <v>131</v>
+      </c>
+      <c r="I38" t="s">
+        <v>173</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" t="s">
         <v>24</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>24</v>
       </c>
-      <c r="F38" t="s">
-        <v>133</v>
-      </c>
-      <c r="G38" t="s">
-        <v>133</v>
-      </c>
-      <c r="I38" t="s">
-        <v>175</v>
-      </c>
-      <c r="J38" t="s">
-        <v>106</v>
-      </c>
-      <c r="K38" t="s">
+      <c r="F39" t="s">
+        <v>132</v>
+      </c>
+      <c r="G39" t="s">
+        <v>132</v>
+      </c>
+      <c r="I39" t="s">
+        <v>174</v>
+      </c>
+      <c r="J39" t="s">
+        <v>105</v>
+      </c>
+      <c r="K39" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
-      <c r="A40" t="s">
-        <v>85</v>
-      </c>
-      <c r="E40" t="s">
-        <v>221</v>
-      </c>
-      <c r="G40" t="s">
+    <row r="41" spans="1:11">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" t="s">
+        <v>218</v>
+      </c>
+      <c r="G41" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="E43" t="s">
+        <v>219</v>
+      </c>
+      <c r="G43" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" t="s">
-        <v>85</v>
-      </c>
-      <c r="E42" t="s">
-        <v>222</v>
-      </c>
-      <c r="G42" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="A44" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" t="s">
-        <v>181</v>
-      </c>
-      <c r="C44" t="s">
-        <v>78</v>
-      </c>
-      <c r="D44" t="s">
-        <v>182</v>
-      </c>
-      <c r="E44" t="s">
-        <v>182</v>
-      </c>
-      <c r="F44" t="s">
-        <v>183</v>
-      </c>
-      <c r="G44" t="s">
-        <v>183</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="J44" t="s">
-        <v>185</v>
-      </c>
-      <c r="K44" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2636,31 +2677,31 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>186</v>
+        <v>231</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D45" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E45" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="F45" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="G45" t="s">
-        <v>188</v>
-      </c>
-      <c r="I45" t="s">
-        <v>189</v>
+        <v>181</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="J45" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="K45" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2668,31 +2709,31 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D46" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="E46" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="F46" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="G46" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I46" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="J46" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="K46" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2700,31 +2741,31 @@
         <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
+        <v>189</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D47" t="s">
-        <v>151</v>
+        <v>190</v>
       </c>
       <c r="E47" t="s">
-        <v>151</v>
+        <v>190</v>
       </c>
       <c r="F47" t="s">
-        <v>120</v>
+        <v>191</v>
       </c>
       <c r="G47" t="s">
-        <v>120</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>107</v>
+        <v>191</v>
+      </c>
+      <c r="I47" t="s">
+        <v>192</v>
+      </c>
+      <c r="J47" t="s">
+        <v>193</v>
+      </c>
+      <c r="K47" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2732,31 +2773,31 @@
         <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>196</v>
+        <v>67</v>
       </c>
       <c r="C48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D48" t="s">
-        <v>197</v>
+        <v>150</v>
       </c>
       <c r="E48" t="s">
-        <v>197</v>
+        <v>150</v>
       </c>
       <c r="F48" t="s">
-        <v>198</v>
+        <v>119</v>
       </c>
       <c r="G48" t="s">
-        <v>198</v>
+        <v>119</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>199</v>
+        <v>168</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2764,31 +2805,31 @@
         <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D49" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E49" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="F49" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="G49" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2796,31 +2837,31 @@
         <v>44</v>
       </c>
       <c r="B50" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D50" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="E50" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="F50" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="G50" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="J50" t="s">
-        <v>210</v>
-      </c>
-      <c r="K50" t="s">
-        <v>210</v>
+        <v>202</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2828,31 +2869,31 @@
         <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D51" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="E51" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="F51" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="G51" t="s">
-        <v>213</v>
-      </c>
-      <c r="I51" t="s">
-        <v>214</v>
+        <v>206</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="J51" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="K51" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2860,31 +2901,63 @@
         <v>44</v>
       </c>
       <c r="B52" t="s">
+        <v>209</v>
+      </c>
+      <c r="C52" t="s">
+        <v>77</v>
+      </c>
+      <c r="D52" t="s">
+        <v>210</v>
+      </c>
+      <c r="E52" t="s">
+        <v>210</v>
+      </c>
+      <c r="F52" t="s">
+        <v>211</v>
+      </c>
+      <c r="G52" t="s">
+        <v>211</v>
+      </c>
+      <c r="I52" t="s">
+        <v>212</v>
+      </c>
+      <c r="J52" t="s">
+        <v>213</v>
+      </c>
+      <c r="K52" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" t="s">
+        <v>230</v>
+      </c>
+      <c r="C53" t="s">
+        <v>77</v>
+      </c>
+      <c r="D53" t="s">
+        <v>214</v>
+      </c>
+      <c r="E53" t="s">
+        <v>214</v>
+      </c>
+      <c r="F53" t="s">
+        <v>215</v>
+      </c>
+      <c r="G53" t="s">
+        <v>215</v>
+      </c>
+      <c r="I53" t="s">
         <v>216</v>
       </c>
-      <c r="C52" t="s">
-        <v>78</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="J53" t="s">
         <v>217</v>
       </c>
-      <c r="E52" t="s">
+      <c r="K53" t="s">
         <v>217</v>
-      </c>
-      <c r="F52" t="s">
-        <v>218</v>
-      </c>
-      <c r="G52" t="s">
-        <v>218</v>
-      </c>
-      <c r="I52" t="s">
-        <v>219</v>
-      </c>
-      <c r="J52" t="s">
-        <v>220</v>
-      </c>
-      <c r="K52" t="s">
-        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>